<commit_message>
Some conversations and Acceptance tests added to User Stories
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -1,27 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Documents/Eclipse Java/Agile_Development_Project1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD95A56-537E-2B40-86D2-E6C28EF88CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Agile User Stories" sheetId="1" r:id="rId4"/>
+    <sheet name="Agile User Stories" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName localSheetId="0" name="YesNo">#REF!</definedName>
-    <definedName localSheetId="0" name="Priority">'Agile User Stories'!$J$4:$J$25</definedName>
-    <definedName localSheetId="0" name="Status">'Agile User Stories'!$K$4:$K$25</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_B0192A1B_C231_4E6E_8016_635727756B48_.wvu.FilterData">'Agile User Stories'!$A$2:$P$25</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_C48613A2_CEF0_4133_8558_F313CB0F2FEB_.wvu.FilterData">'Agile User Stories'!$B$2:$H$28</definedName>
+    <definedName name="Priority" localSheetId="0">'Agile User Stories'!$J$4:$J$25</definedName>
+    <definedName name="Status" localSheetId="0">'Agile User Stories'!$K$4:$K$25</definedName>
+    <definedName name="YesNo" localSheetId="0">#REF!</definedName>
+    <definedName name="Z_B0192A1B_C231_4E6E_8016_635727756B48_.wvu.FilterData" localSheetId="0" hidden="1">'Agile User Stories'!$A$2:$P$25</definedName>
+    <definedName name="Z_C48613A2_CEF0_4133_8558_F313CB0F2FEB_.wvu.FilterData" localSheetId="0" hidden="1">'Agile User Stories'!$B$2:$H$28</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{C48613A2-CEF0-4133-8558-F313CB0F2FEB}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{B0192A1B-C231-4E6E-8016-635727756B48}" name="Filter 1"/>
+    <customWorkbookView name="Filter 2" guid="{C48613A2-CEF0-4133-8558-F313CB0F2FEB}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{B0192A1B-C231-4E6E-8016-635727756B48}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>USER STORIES</t>
   </si>
@@ -117,86 +137,140 @@
   </si>
   <si>
     <t>As a programmer, I would like to create a webpage as the main interface to allow the user easy and effective access to all the data.</t>
+  </si>
+  <si>
+    <t>- Stored as the first 3 digits of DRG Definition 
+- Between 000 and 999
+- Add user input validation on front end
+- Separate from Description when using Search (radio buttons)
+- Shows only entries with the exact number</t>
+  </si>
+  <si>
+    <t>- Test that the user input is only 3 digits
+- Test that the input does not include special characters
+- Test that the input field is not empty
+- Test that an incorrect input shows a message</t>
+  </si>
+  <si>
+    <t>- Stored as DRG Definition
+- Description might not be exact
+- not case sensitive
+- If no exact result based on lexical similarity
+- Ignore whitespace</t>
+  </si>
+  <si>
+    <t>- Test that the input field is not empty
+- Test finding an entry with exact wording
+- Test finding a close match is the entry does not match
+- Test that a message is generated if there are no matches</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="20.0"/>
+      <sz val="20"/>
       <color rgb="FF7F7F7F"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="0"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="22.0"/>
+      <sz val="22"/>
       <color theme="0"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -218,17 +292,26 @@
     </fill>
   </fills>
   <borders count="11">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -243,27 +326,34 @@
       <bottom style="thin">
         <color rgb="FFBFBFBF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FFBFBFBF"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FFBFBFBF"/>
       </top>
       <bottom style="thin">
         <color rgb="FFBFBFBF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -278,6 +368,7 @@
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -286,125 +377,141 @@
       <right style="thin">
         <color rgb="FFBFBFBF"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FFBFBFBF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="33">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -594,36 +701,39 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFF2F2F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.29"/>
-    <col customWidth="1" min="2" max="2" width="10.86"/>
-    <col customWidth="1" min="3" max="3" width="110.57"/>
-    <col customWidth="1" min="4" max="6" width="15.29"/>
-    <col customWidth="1" min="7" max="7" width="20.14"/>
-    <col customWidth="1" min="8" max="8" width="34.71"/>
-    <col customWidth="1" min="9" max="9" width="3.29"/>
-    <col customWidth="1" min="10" max="11" width="17.86"/>
-    <col customWidth="1" min="12" max="12" width="3.29"/>
-    <col customWidth="1" min="13" max="16" width="10.86"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="110.5" customWidth="1"/>
+    <col min="4" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="57.1640625" customWidth="1"/>
+    <col min="8" max="8" width="60.6640625" customWidth="1"/>
+    <col min="9" max="9" width="3.33203125" customWidth="1"/>
+    <col min="10" max="11" width="17.83203125" customWidth="1"/>
+    <col min="12" max="12" width="3.33203125" customWidth="1"/>
+    <col min="13" max="16" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="49.5" customHeight="1">
+    <row r="1" spans="1:16" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -643,7 +753,7 @@
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
     </row>
-    <row r="2" ht="34.5" customHeight="1">
+    <row r="2" spans="1:16" ht="50" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -675,709 +785,721 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" ht="34.5" customHeight="1">
+    <row r="3" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="11">
-        <f t="shared" ref="B3:B28" si="1">ROW()-2</f>
+        <f t="shared" ref="B3:B28" si="0">ROW()-2</f>
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13">
-        <v>9.0</v>
-      </c>
-      <c r="E3" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="14">
-        <f t="shared" ref="F3:F26" si="2">ROUND((D3/E3),0)</f>
+      <c r="D3" s="28">
         <v>9</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="E3" s="29">
+        <v>1</v>
+      </c>
+      <c r="F3" s="29">
+        <f t="shared" ref="F3:F26" si="1">ROUND((D3/E3),0)</f>
+        <v>9</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>33</v>
+      </c>
       <c r="I3" s="9"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
       <c r="L3" s="1"/>
       <c r="M3" s="10"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" ht="34.5" customHeight="1">
+    <row r="4" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14">
-        <v>10.0</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="14">
-        <f t="shared" si="2"/>
+      <c r="D4" s="29">
         <v>10</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="E4" s="29">
+        <v>1</v>
+      </c>
+      <c r="F4" s="29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>35</v>
+      </c>
       <c r="I4" s="9"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="15"/>
       <c r="L4" s="1"/>
       <c r="M4" s="10"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" ht="34.5" customHeight="1">
+    <row r="5" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14">
-        <v>10.0</v>
-      </c>
-      <c r="E5" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="14">
-        <f t="shared" si="2"/>
+      <c r="D5" s="29">
         <v>10</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="E5" s="29">
+        <v>1</v>
+      </c>
+      <c r="F5" s="29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>35</v>
+      </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="1"/>
       <c r="M5" s="10"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" ht="34.5" customHeight="1">
+    <row r="6" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="14">
-        <v>7.0</v>
-      </c>
-      <c r="E6" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="F6" s="14">
-        <f t="shared" si="2"/>
+      <c r="D6" s="29">
+        <v>7</v>
+      </c>
+      <c r="E6" s="29">
+        <v>4</v>
+      </c>
+      <c r="F6" s="29">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="1"/>
       <c r="M6" s="10"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" ht="34.5" customHeight="1">
+    <row r="7" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="14">
-        <v>9.0</v>
-      </c>
-      <c r="E7" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="F7" s="14">
-        <f t="shared" si="2"/>
+      <c r="D7" s="29">
+        <v>9</v>
+      </c>
+      <c r="E7" s="29">
+        <v>4</v>
+      </c>
+      <c r="F7" s="29">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="1"/>
       <c r="M7" s="10"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" ht="34.5" customHeight="1">
+    <row r="8" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="14">
-        <v>6.0</v>
-      </c>
-      <c r="E8" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="F8" s="14">
-        <f t="shared" si="2"/>
+      <c r="D8" s="29">
+        <v>6</v>
+      </c>
+      <c r="E8" s="29">
+        <v>2</v>
+      </c>
+      <c r="F8" s="29">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="17"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="1"/>
       <c r="M8" s="10"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" ht="34.5" customHeight="1">
+    <row r="9" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="14">
-        <v>6.0</v>
-      </c>
-      <c r="E9" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="F9" s="14">
-        <f t="shared" si="2"/>
+      <c r="D9" s="29">
+        <v>6</v>
+      </c>
+      <c r="E9" s="29">
+        <v>2</v>
+      </c>
+      <c r="F9" s="29">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="1"/>
       <c r="M9" s="10"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" ht="34.5" customHeight="1">
+    <row r="10" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="14">
-        <v>8.0</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="F10" s="14">
-        <f t="shared" si="2"/>
+      <c r="D10" s="29">
         <v>8</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="E10" s="29">
+        <v>1</v>
+      </c>
+      <c r="F10" s="29">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="1"/>
       <c r="M10" s="10"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" ht="34.5" customHeight="1">
+    <row r="11" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="14">
-        <v>8.0</v>
-      </c>
-      <c r="E11" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="F11" s="14">
-        <f t="shared" si="2"/>
+      <c r="D11" s="29">
         <v>8</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="E11" s="29">
+        <v>1</v>
+      </c>
+      <c r="F11" s="29">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="1"/>
       <c r="M11" s="10"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" ht="34.5" customHeight="1">
+    <row r="12" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="14">
-        <v>10.0</v>
-      </c>
-      <c r="E12" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="F12" s="14">
-        <f t="shared" si="2"/>
+      <c r="D12" s="29">
+        <v>10</v>
+      </c>
+      <c r="E12" s="29">
         <v>3</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="F12" s="29">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="1"/>
       <c r="M12" s="10"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" ht="34.5" customHeight="1">
+    <row r="13" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="14">
-        <v>5.0</v>
-      </c>
-      <c r="E13" s="14">
-        <v>7.0</v>
-      </c>
-      <c r="F13" s="14">
-        <f t="shared" si="2"/>
+      <c r="D13" s="29">
+        <v>5</v>
+      </c>
+      <c r="E13" s="29">
+        <v>7</v>
+      </c>
+      <c r="F13" s="29">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="1"/>
       <c r="M13" s="10"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" ht="34.5" customHeight="1">
+    <row r="14" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="E14" s="14">
-        <v>6.0</v>
-      </c>
-      <c r="F14" s="14">
-        <f t="shared" si="2"/>
+      <c r="D14" s="29">
+        <v>4</v>
+      </c>
+      <c r="E14" s="29">
+        <v>6</v>
+      </c>
+      <c r="F14" s="29">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
       <c r="L14" s="1"/>
       <c r="M14" s="10"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" ht="34.5" customHeight="1">
+    <row r="15" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="14">
-        <v>7.0</v>
-      </c>
-      <c r="E15" s="14">
-        <v>5.0</v>
-      </c>
-      <c r="F15" s="14">
-        <f t="shared" si="2"/>
+      <c r="D15" s="29">
+        <v>7</v>
+      </c>
+      <c r="E15" s="29">
+        <v>5</v>
+      </c>
+      <c r="F15" s="29">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="1"/>
       <c r="M15" s="10"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" ht="34.5" customHeight="1">
+    <row r="16" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="14">
-        <v>10.0</v>
-      </c>
-      <c r="E16" s="14">
-        <v>6.0</v>
-      </c>
-      <c r="F16" s="14">
-        <f t="shared" si="2"/>
+      <c r="D16" s="29">
+        <v>10</v>
+      </c>
+      <c r="E16" s="29">
+        <v>6</v>
+      </c>
+      <c r="F16" s="29">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
       <c r="L16" s="1"/>
       <c r="M16" s="10"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" ht="34.5" customHeight="1">
+    <row r="17" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="E17" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="F17" s="14">
-        <f t="shared" si="2"/>
+      <c r="D17" s="29">
+        <v>2</v>
+      </c>
+      <c r="E17" s="29">
+        <v>2</v>
+      </c>
+      <c r="F17" s="29">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="1"/>
       <c r="M17" s="10"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" ht="34.5" customHeight="1">
+    <row r="18" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="E18" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="F18" s="14">
-        <f t="shared" si="2"/>
+      <c r="D18" s="29">
+        <v>3</v>
+      </c>
+      <c r="E18" s="29">
+        <v>3</v>
+      </c>
+      <c r="F18" s="29">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
       <c r="L18" s="1"/>
       <c r="M18" s="10"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" ht="34.5" customHeight="1">
+    <row r="19" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="E19" s="14">
-        <v>5.0</v>
-      </c>
-      <c r="F19" s="14">
-        <f t="shared" si="2"/>
+      <c r="D19" s="29">
+        <v>4</v>
+      </c>
+      <c r="E19" s="29">
+        <v>5</v>
+      </c>
+      <c r="F19" s="29">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
       <c r="I19" s="9"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
       <c r="L19" s="1"/>
       <c r="M19" s="10"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" ht="34.5" customHeight="1">
+    <row r="20" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14" t="str">
-        <f t="shared" si="2"/>
+      <c r="D20" s="29">
+        <v>1</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
       <c r="L20" s="1"/>
       <c r="M20" s="10"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" ht="34.5" customHeight="1">
+    <row r="21" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14" t="str">
-        <f t="shared" si="2"/>
+      <c r="D21" s="29">
+        <v>1</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
       <c r="L21" s="1"/>
       <c r="M21" s="10"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
     </row>
-    <row r="22" ht="34.5" customHeight="1">
+    <row r="22" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14" t="str">
-        <f t="shared" si="2"/>
+      <c r="D22" s="29">
+        <v>1</v>
+      </c>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
       <c r="L22" s="1"/>
       <c r="M22" s="10"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" ht="34.5" customHeight="1">
+    <row r="23" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14" t="str">
-        <f t="shared" si="2"/>
+      <c r="D23" s="29">
+        <v>1</v>
+      </c>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
       <c r="L23" s="1"/>
       <c r="M23" s="10"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" ht="34.5" customHeight="1">
+    <row r="24" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="E24" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="F24" s="14">
-        <f t="shared" si="2"/>
+      <c r="D24" s="29">
         <v>3</v>
       </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="E24" s="29">
+        <v>1</v>
+      </c>
+      <c r="F24" s="29">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
       <c r="L24" s="1"/>
       <c r="M24" s="10"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" ht="34.5" customHeight="1">
+    <row r="25" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="E25" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="F25" s="14">
-        <f t="shared" si="2"/>
+      <c r="D25" s="29">
+        <v>3</v>
+      </c>
+      <c r="E25" s="29">
         <v>2</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="F25" s="29">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
       <c r="L25" s="1"/>
       <c r="M25" s="10"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" ht="34.5" customHeight="1">
+    <row r="26" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="14">
-        <v>10.0</v>
-      </c>
-      <c r="E26" s="14">
-        <v>5.0</v>
-      </c>
-      <c r="F26" s="14">
-        <f t="shared" si="2"/>
+      <c r="D26" s="29">
+        <v>10</v>
+      </c>
+      <c r="E26" s="29">
+        <v>5</v>
+      </c>
+      <c r="F26" s="29">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
       <c r="I26" s="9"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1387,39 +1509,39 @@
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" ht="34.5" customHeight="1">
+    <row r="27" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
     </row>
-    <row r="28" ht="34.5" customHeight="1">
+    <row r="28" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -1429,7 +1551,7 @@
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" ht="9.75" customHeight="1">
+    <row r="29" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="5"/>
@@ -1447,33 +1569,33 @@
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
     </row>
-    <row r="30" ht="49.5" customHeight="1">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="29"/>
-    </row>
-    <row r="31" ht="12.75" customHeight="1">
+    <row r="30" spans="1:16" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="19"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+    </row>
+    <row r="31" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -1483,15 +1605,15 @@
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" ht="12.75" customHeight="1">
+    <row r="32" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -1501,7 +1623,7 @@
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" ht="12.75" customHeight="1">
+    <row r="33" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="5"/>
@@ -1519,7 +1641,7 @@
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" ht="12.75" customHeight="1">
+    <row r="34" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="5"/>
@@ -1537,7 +1659,7 @@
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
     </row>
-    <row r="35" ht="12.75" customHeight="1">
+    <row r="35" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="5"/>
@@ -1555,7 +1677,7 @@
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
-    <row r="36" ht="12.75" customHeight="1">
+    <row r="36" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="5"/>
@@ -1573,7 +1695,7 @@
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" ht="12.75" customHeight="1">
+    <row r="37" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="5"/>
@@ -1591,7 +1713,7 @@
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
-    <row r="38" ht="12.75" customHeight="1">
+    <row r="38" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="5"/>
@@ -1609,7 +1731,7 @@
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
     </row>
-    <row r="39" ht="12.75" customHeight="1">
+    <row r="39" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="5"/>
@@ -1627,7 +1749,7 @@
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" ht="12.75" customHeight="1">
+    <row r="40" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="5"/>
@@ -1645,7 +1767,7 @@
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" ht="12.75" customHeight="1">
+    <row r="41" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="5"/>
@@ -1663,7 +1785,7 @@
       <c r="O41" s="5"/>
       <c r="P41" s="5"/>
     </row>
-    <row r="42" ht="12.75" customHeight="1">
+    <row r="42" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="5"/>
@@ -1681,7 +1803,7 @@
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
     </row>
-    <row r="43" ht="12.75" customHeight="1">
+    <row r="43" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="5"/>
@@ -1699,7 +1821,7 @@
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
     </row>
-    <row r="44" ht="12.75" customHeight="1">
+    <row r="44" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="5"/>
@@ -1717,7 +1839,7 @@
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
     </row>
-    <row r="45" ht="12.75" customHeight="1">
+    <row r="45" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="5"/>
@@ -1735,7 +1857,7 @@
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
     </row>
-    <row r="46" ht="12.75" customHeight="1">
+    <row r="46" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="5"/>
@@ -1753,7 +1875,7 @@
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
     </row>
-    <row r="47" ht="12.75" customHeight="1">
+    <row r="47" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="5"/>
@@ -1771,7 +1893,7 @@
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
     </row>
-    <row r="48" ht="12.75" customHeight="1">
+    <row r="48" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="5"/>
@@ -1789,7 +1911,7 @@
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
     </row>
-    <row r="49" ht="12.75" customHeight="1">
+    <row r="49" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="5"/>
@@ -1807,7 +1929,7 @@
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
     </row>
-    <row r="50" ht="12.75" customHeight="1">
+    <row r="50" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="5"/>
@@ -1828,15 +1950,17 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{C48613A2-CEF0-4133-8558-F313CB0F2FEB}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$B$2:$H$28">
-        <sortState ref="B2:H28">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="B2:H28" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H28">
           <sortCondition descending="1" ref="D2:D28"/>
         </sortState>
       </autoFilter>
     </customSheetView>
     <customSheetView guid="{B0192A1B-C231-4E6E-8016-635727756B48}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$A$2:$P$25">
-        <sortState ref="A2:P25">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:P25" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P25">
           <sortCondition descending="1" ref="D2:D25"/>
           <sortCondition ref="E2:E25"/>
         </sortState>
@@ -1846,9 +1970,7 @@
   <mergeCells count="1">
     <mergeCell ref="B30:H30"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.3" footer="0.0" header="0.0" left="0.3" right="0.3" top="0.3"/>
+  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup fitToHeight="0" orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
User story added (integration)
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Documents/Eclipse Java/Agile_Development_Project1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD95A56-537E-2B40-86D2-E6C28EF88CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21EC2F4-9229-6547-8B61-62991BCA4A59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{B0192A1B-C231-4E6E-8016-635727756B48}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{C48613A2-CEF0-4133-8558-F313CB0F2FEB}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{B0192A1B-C231-4E6E-8016-635727756B48}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>USER STORIES</t>
   </si>
@@ -163,6 +163,24 @@
 - Test finding an entry with exact wording
 - Test finding a close match is the entry does not match
 - Test that a message is generated if there are no matches</t>
+  </si>
+  <si>
+    <t>As a programmer, I want to integrate the database, backend and frontend to allaw the user a seamless experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Using MySQL database hosted on Azure
+- Whole project deployed to Azure with Web app
+- Java EE for backend, developed in EclipseEE
+- For development purposes hosted on Apache Tomcat servers
+- Integration between frontend and backend with JSP files
+- Frontend in HTML and CSS using a Bootstrap template
+</t>
+  </si>
+  <si>
+    <t>- Test that the database is available
+- Test that backend connects successfully to the database
+- Test that user input can be called in the JSP file and used in the Java file
+- Test the frontend works and is displayed correctly</t>
   </si>
 </sst>
 </file>
@@ -401,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -493,6 +511,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,9 +738,9 @@
   </sheetPr>
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -801,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="29">
-        <f t="shared" ref="F3:F26" si="1">ROUND((D3/E3),0)</f>
+        <f t="shared" ref="F3:F27" si="1">ROUND((D3/E3),0)</f>
         <v>9</v>
       </c>
       <c r="G3" s="23" t="s">
@@ -1509,18 +1533,31 @@
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" ht="112" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="11">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
+      <c r="C27" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="33">
+        <v>10</v>
+      </c>
+      <c r="E27" s="33">
+        <v>7</v>
+      </c>
+      <c r="F27" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>38</v>
+      </c>
       <c r="I27" s="5"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -1949,20 +1986,20 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C48613A2-CEF0-4133-8558-F313CB0F2FEB}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="B2:H28" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H28">
-          <sortCondition descending="1" ref="D2:D28"/>
-        </sortState>
-      </autoFilter>
-    </customSheetView>
     <customSheetView guid="{B0192A1B-C231-4E6E-8016-635727756B48}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A2:P25" xr:uid="{00000000-0000-0000-0000-000000000000}">
         <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P25">
           <sortCondition descending="1" ref="D2:D25"/>
           <sortCondition ref="E2:E25"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{C48613A2-CEF0-4133-8558-F313CB0F2FEB}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="B2:H28" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H28">
+          <sortCondition descending="1" ref="D2:D28"/>
         </sortState>
       </autoFilter>
     </customSheetView>

</xml_diff>